<commit_message>
fix schematic and BOM
</commit_message>
<xml_diff>
--- a/boards/Distribution/Distribution_BOM.xlsx
+++ b/boards/Distribution/Distribution_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lipoy\Dropbox\develop\StackChanPwd\StackChanPwd\boards\Distribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FD9419-07E4-4ACC-835D-6DA112B983F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EA4865-2715-4174-ADDB-2739506031EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{77968056-1277-4E85-A75B-247B36802C55}"/>
   </bookViews>
@@ -115,18 +115,9 @@
     <t>R2</t>
   </si>
   <si>
-    <t>330Ω, class F</t>
-  </si>
-  <si>
-    <t>10-ERJ-U03F3300VCT-ND</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
-    <t>10Ω, class F</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -139,7 +130,19 @@
     <t>811-2072-1-ND</t>
   </si>
   <si>
-    <t>10-ERJ-U03F10R0VCT-ND</t>
+    <t>220Ω, class F</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>22Ω, class F</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>10-ERJ-U03F2200VCT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>10-ERJ-U03F22R0VCT-ND</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -1121,9 +1124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BCE1B38-FD18-4009-A3C8-7E3EFD726F9A}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1286,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
@@ -1299,18 +1300,18 @@
         <v>11</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>10</v>
@@ -1328,16 +1329,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1345,7 +1346,7 @@
         <v>11</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>